<commit_message>
somewhat change text; change xlsx
</commit_message>
<xml_diff>
--- a/src/assets/Corona_Dashboard_RawData - KKH_ITS.xlsx
+++ b/src/assets/Corona_Dashboard_RawData - KKH_ITS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kainagel/git/matsim-all/covid-sim/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B31C49-9C69-CD4C-B3B0-25A38CE2675B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4ED0C6-FD07-B14E-9DE6-7E09C19590AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="38400" windowHeight="23440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5028,7 +5028,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5756,8 +5756,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>

</xml_diff>